<commit_message>
upload IDPT version 1.0 for release + publication outputs.
</commit_message>
<xml_diff>
--- a/publication/analyses/outputs/field_dependent_effects/gdpt_fit_results.xlsx
+++ b/publication/analyses/outputs/field_dependent_effects/gdpt_fit_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,25 +480,25 @@
         <v>-48.09999999999999</v>
       </c>
       <c r="B2" t="n">
-        <v>3.653404140424973e-06</v>
+        <v>2.80738880071268e-06</v>
       </c>
       <c r="C2" t="n">
-        <v>-47.80828328593272</v>
+        <v>-47.80829537787529</v>
       </c>
       <c r="D2" t="n">
-        <v>88.5779037566686</v>
+        <v>90.82539594511528</v>
       </c>
       <c r="E2" t="n">
-        <v>770.8963676195477</v>
+        <v>827.8255058766849</v>
       </c>
       <c r="F2" t="n">
-        <v>1.179303168920434</v>
+        <v>0.7416168208955816</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5457427306874374</v>
+        <v>0.4522805940438833</v>
       </c>
       <c r="H2" t="n">
-        <v>91</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
@@ -506,25 +506,25 @@
         <v>-43.09999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>1.8680751068696e-06</v>
+        <v>2.318331709998723e-06</v>
       </c>
       <c r="C3" t="n">
-        <v>-43.14635805364571</v>
+        <v>-43.14635803198964</v>
       </c>
       <c r="D3" t="n">
-        <v>88.21044322604301</v>
+        <v>91.0687371765809</v>
       </c>
       <c r="E3" t="n">
-        <v>733.624420698693</v>
+        <v>827.6612304733294</v>
       </c>
       <c r="F3" t="n">
-        <v>1.176132577344591</v>
+        <v>0.8247158231892143</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5360954451797328</v>
+        <v>0.7149604635334523</v>
       </c>
       <c r="H3" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -532,25 +532,25 @@
         <v>-38.09999999999999</v>
       </c>
       <c r="B4" t="n">
-        <v>7.255190991212597e-07</v>
+        <v>1.997579738166616e-06</v>
       </c>
       <c r="C4" t="n">
-        <v>-37.68518844029698</v>
+        <v>-37.68518843851263</v>
       </c>
       <c r="D4" t="n">
-        <v>146.3714630657717</v>
+        <v>90.78470942882738</v>
       </c>
       <c r="E4" t="n">
-        <v>709.633676277357</v>
+        <v>828.8377067354797</v>
       </c>
       <c r="F4" t="n">
-        <v>1.750913184157291</v>
+        <v>0.6584141975665039</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5853805038997958</v>
+        <v>0.7484436890083045</v>
       </c>
       <c r="H4" t="n">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
@@ -558,25 +558,25 @@
         <v>-33.09999999999999</v>
       </c>
       <c r="B5" t="n">
-        <v>-8.976785148096682e-07</v>
+        <v>2.123849906631237e-06</v>
       </c>
       <c r="C5" t="n">
-        <v>-32.98388033301515</v>
+        <v>-32.98388033521915</v>
       </c>
       <c r="D5" t="n">
-        <v>87.07059651952528</v>
+        <v>90.90222861986571</v>
       </c>
       <c r="E5" t="n">
-        <v>709.5294438146223</v>
+        <v>829.8173284104438</v>
       </c>
       <c r="F5" t="n">
-        <v>1.308543170843081</v>
+        <v>0.9791104747640316</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5490247282263772</v>
+        <v>0.6965302356205293</v>
       </c>
       <c r="H5" t="n">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
         <v>-28.09999999999999</v>
       </c>
       <c r="B6" t="n">
-        <v>-2.157253854231768e-06</v>
+        <v>1.370316468192153e-06</v>
       </c>
       <c r="C6" t="n">
-        <v>-28.40995576800577</v>
+        <v>-28.40995576350308</v>
       </c>
       <c r="D6" t="n">
-        <v>87.00993476288129</v>
+        <v>90.65356287048206</v>
       </c>
       <c r="E6" t="n">
-        <v>826.080936604742</v>
+        <v>830.2837598993303</v>
       </c>
       <c r="F6" t="n">
-        <v>1.019808237786181</v>
+        <v>0.793987156701334</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5242580860025041</v>
+        <v>0.6679291429363076</v>
       </c>
       <c r="H6" t="n">
-        <v>185</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
@@ -610,25 +610,25 @@
         <v>-23.09999999999999</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.227041973078653e-06</v>
+        <v>1.336500239866959e-06</v>
       </c>
       <c r="C7" t="n">
-        <v>-22.86769736418611</v>
+        <v>-22.86769729371633</v>
       </c>
       <c r="D7" t="n">
-        <v>86.02343577742212</v>
+        <v>90.49122637440026</v>
       </c>
       <c r="E7" t="n">
-        <v>826.4253593574985</v>
+        <v>830.6334606269025</v>
       </c>
       <c r="F7" t="n">
-        <v>1.004776217349364</v>
+        <v>0.8056979721817132</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6343985567085602</v>
+        <v>0.6697773104231175</v>
       </c>
       <c r="H7" t="n">
-        <v>209</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
@@ -636,25 +636,25 @@
         <v>-18.09999999999999</v>
       </c>
       <c r="B8" t="n">
-        <v>-2.235160629921176e-06</v>
+        <v>6.339378657590692e-07</v>
       </c>
       <c r="C8" t="n">
-        <v>-18.20520396641349</v>
+        <v>-18.20520397000868</v>
       </c>
       <c r="D8" t="n">
-        <v>85.62491873279768</v>
+        <v>90.31453946716641</v>
       </c>
       <c r="E8" t="n">
-        <v>826.7303719105375</v>
+        <v>830.7242974601622</v>
       </c>
       <c r="F8" t="n">
-        <v>1.05707573174077</v>
+        <v>0.9503593598754119</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6896025184706505</v>
+        <v>0.5999388550668032</v>
       </c>
       <c r="H8" t="n">
-        <v>212</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9">
@@ -662,25 +662,25 @@
         <v>-13.09999999999999</v>
       </c>
       <c r="B9" t="n">
-        <v>-2.046731857223729e-06</v>
+        <v>-3.923298197014747e-07</v>
       </c>
       <c r="C9" t="n">
-        <v>-13.53538260579001</v>
+        <v>-13.53538203551962</v>
       </c>
       <c r="D9" t="n">
-        <v>87.96732686196748</v>
+        <v>90.40648246556162</v>
       </c>
       <c r="E9" t="n">
-        <v>827.1920289909676</v>
+        <v>831.0423878309792</v>
       </c>
       <c r="F9" t="n">
-        <v>1.102586660891152</v>
+        <v>1.291263089249161</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7220895409710262</v>
+        <v>0.5191800489044687</v>
       </c>
       <c r="H9" t="n">
-        <v>202</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
@@ -688,25 +688,25 @@
         <v>-8.099999999999994</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.389830428678122e-06</v>
+        <v>-2.201736949984444e-07</v>
       </c>
       <c r="C10" t="n">
-        <v>-8.412366556792776</v>
+        <v>-8.412366102243347</v>
       </c>
       <c r="D10" t="n">
-        <v>87.60784133680548</v>
+        <v>90.13248741757634</v>
       </c>
       <c r="E10" t="n">
-        <v>772.6855271073306</v>
+        <v>830.8335811319689</v>
       </c>
       <c r="F10" t="n">
-        <v>1.544017991615241</v>
+        <v>1.454014770682649</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6861266829598519</v>
+        <v>0.6738613806618279</v>
       </c>
       <c r="H10" t="n">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11">
@@ -714,25 +714,25 @@
         <v>-3.099999999999994</v>
       </c>
       <c r="B11" t="n">
-        <v>4.785425400593292e-06</v>
+        <v>-1.780561801267056e-06</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.162115879123987</v>
+        <v>-4.162115875665234</v>
       </c>
       <c r="D11" t="n">
-        <v>87.31470706420379</v>
+        <v>186.8533940033314</v>
       </c>
       <c r="E11" t="n">
-        <v>772.5184113857581</v>
+        <v>830.5485616267192</v>
       </c>
       <c r="F11" t="n">
-        <v>2.730340097670982</v>
+        <v>1.92309375837692</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7090236505832517</v>
+        <v>0.6170306428121161</v>
       </c>
       <c r="H11" t="n">
-        <v>193</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
@@ -740,25 +740,25 @@
         <v>1.900000000000006</v>
       </c>
       <c r="B12" t="n">
-        <v>-6.2900836277428e-06</v>
+        <v>-1.45642546286813e-06</v>
       </c>
       <c r="C12" t="n">
         <v>1.5</v>
       </c>
       <c r="D12" t="n">
-        <v>87.19636101622038</v>
+        <v>89.70839706418597</v>
       </c>
       <c r="E12" t="n">
-        <v>772.5743203653634</v>
+        <v>771.5078743507485</v>
       </c>
       <c r="F12" t="n">
-        <v>1.552831161157699</v>
+        <v>2.317933490908868</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4819775395574681</v>
+        <v>0.5909648256944725</v>
       </c>
       <c r="H12" t="n">
-        <v>192</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13">
@@ -766,25 +766,25 @@
         <v>6.900000000000006</v>
       </c>
       <c r="B13" t="n">
-        <v>-9.740956411073031e-06</v>
+        <v>-2.597801391765845e-06</v>
       </c>
       <c r="C13" t="n">
-        <v>6.883590418386336</v>
+        <v>6.883590571785827</v>
       </c>
       <c r="D13" t="n">
-        <v>206.6524249297134</v>
+        <v>90.01028177563565</v>
       </c>
       <c r="E13" t="n">
-        <v>654.4652123759919</v>
+        <v>771.6986054665356</v>
       </c>
       <c r="F13" t="n">
-        <v>1.723151010737687</v>
+        <v>0.9630759392654894</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3342940587377499</v>
+        <v>0.6927977533583594</v>
       </c>
       <c r="H13" t="n">
-        <v>43</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
@@ -792,25 +792,25 @@
         <v>11.90000000000001</v>
       </c>
       <c r="B14" t="n">
-        <v>-8.391794742983474e-06</v>
+        <v>-3.972583130352006e-06</v>
       </c>
       <c r="C14" t="n">
-        <v>12.29422759640145</v>
+        <v>12.29422759822129</v>
       </c>
       <c r="D14" t="n">
-        <v>206.482725585017</v>
+        <v>90.13215442508441</v>
       </c>
       <c r="E14" t="n">
-        <v>625.8949088113651</v>
+        <v>771.9591986155116</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6804451630503833</v>
+        <v>0.8578763283534891</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7699987839356704</v>
+        <v>0.7300137378305677</v>
       </c>
       <c r="H14" t="n">
-        <v>26</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15">
@@ -818,181 +818,207 @@
         <v>16.90000000000001</v>
       </c>
       <c r="B15" t="n">
-        <v>-7.832174172935491e-06</v>
+        <v>-4.150207436159695e-06</v>
       </c>
       <c r="C15" t="n">
-        <v>17.00709991454513</v>
+        <v>17.00708776609423</v>
       </c>
       <c r="D15" t="n">
-        <v>158.2860404703793</v>
+        <v>90.11881280976174</v>
       </c>
       <c r="E15" t="n">
-        <v>734.7068382277916</v>
+        <v>830.6407109746081</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8453722637138561</v>
+        <v>0.9094950290507534</v>
       </c>
       <c r="G15" t="n">
-        <v>0.6583926700369021</v>
+        <v>0.6966699915145911</v>
       </c>
       <c r="H15" t="n">
-        <v>36</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>26.90000000000001</v>
+        <v>21.90000000000001</v>
       </c>
       <c r="B16" t="n">
-        <v>-9.394125278961196e-06</v>
+        <v>-4.741710607907295e-06</v>
       </c>
       <c r="C16" t="n">
-        <v>27.84517993602329</v>
+        <v>22.14348712706708</v>
       </c>
       <c r="D16" t="n">
-        <v>87.01593297241631</v>
+        <v>90.21794785462249</v>
       </c>
       <c r="E16" t="n">
-        <v>615.7466714501821</v>
+        <v>830.2221608451788</v>
       </c>
       <c r="F16" t="n">
-        <v>1.024800387043638</v>
+        <v>0.8859619568781814</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2934213400644352</v>
+        <v>0.744676304663677</v>
       </c>
       <c r="H16" t="n">
-        <v>26</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>31.90000000000001</v>
+        <v>26.90000000000001</v>
       </c>
       <c r="B17" t="n">
-        <v>-8.247092951252192e-06</v>
+        <v>-5.35908295853718e-06</v>
       </c>
       <c r="C17" t="n">
-        <v>32.6327596643745</v>
+        <v>27.84518183438559</v>
       </c>
       <c r="D17" t="n">
-        <v>86.85018533265635</v>
+        <v>90.18888841688099</v>
       </c>
       <c r="E17" t="n">
-        <v>734.6759949288084</v>
+        <v>829.7983117699556</v>
       </c>
       <c r="F17" t="n">
-        <v>1.127397189014557</v>
+        <v>0.8296708479267555</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7186184135970054</v>
+        <v>0.7849704397612036</v>
       </c>
       <c r="H17" t="n">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>36.90000000000001</v>
+        <v>31.90000000000001</v>
       </c>
       <c r="B18" t="n">
-        <v>-9.346534447767307e-06</v>
+        <v>-5.749188643935305e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>37.69292631543188</v>
+        <v>32.63277172314476</v>
       </c>
       <c r="D18" t="n">
-        <v>86.89998033087674</v>
+        <v>90.15951874917874</v>
       </c>
       <c r="E18" t="n">
-        <v>773.0996886118246</v>
+        <v>772.4037783531151</v>
       </c>
       <c r="F18" t="n">
-        <v>1.229753961965541</v>
+        <v>0.8516371813098846</v>
       </c>
       <c r="G18" t="n">
-        <v>0.7090686377300905</v>
+        <v>0.8454017226245476</v>
       </c>
       <c r="H18" t="n">
-        <v>133</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>41.90000000000001</v>
+        <v>36.90000000000001</v>
       </c>
       <c r="B19" t="n">
-        <v>-9.195955848881288e-06</v>
+        <v>-6.353637337595844e-06</v>
       </c>
       <c r="C19" t="n">
-        <v>42.4389663528382</v>
+        <v>37.69291482618024</v>
       </c>
       <c r="D19" t="n">
-        <v>86.59486943944944</v>
+        <v>90.29657357722289</v>
       </c>
       <c r="E19" t="n">
-        <v>772.2215792022571</v>
+        <v>773.0103223849046</v>
       </c>
       <c r="F19" t="n">
-        <v>1.532047262308794</v>
+        <v>1.018444302602618</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6999987383541481</v>
+        <v>0.8347644503624119</v>
       </c>
       <c r="H19" t="n">
-        <v>133</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>46.90000000000001</v>
+        <v>41.90000000000001</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.089223857124962e-05</v>
+        <v>-5.173322218226858e-06</v>
       </c>
       <c r="C20" t="n">
-        <v>47.73906568297598</v>
+        <v>42.43896635786598</v>
       </c>
       <c r="D20" t="n">
-        <v>86.80773214068127</v>
+        <v>89.88634796144834</v>
       </c>
       <c r="E20" t="n">
-        <v>734.6029182247585</v>
+        <v>772.4977024774959</v>
       </c>
       <c r="F20" t="n">
-        <v>1.417376981945002</v>
+        <v>1.054231890990177</v>
       </c>
       <c r="G20" t="n">
-        <v>0.6178164504321986</v>
+        <v>0.7408134199985423</v>
       </c>
       <c r="H20" t="n">
-        <v>121</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
+        <v>46.90000000000001</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-4.696845708077501e-06</v>
+      </c>
+      <c r="C21" t="n">
+        <v>47.73905463312075</v>
+      </c>
+      <c r="D21" t="n">
+        <v>90.42234393547059</v>
+      </c>
+      <c r="E21" t="n">
+        <v>772.6022991595236</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.8897300773309664</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.6814878313815504</v>
+      </c>
+      <c r="H21" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>51.90000000000001</v>
       </c>
-      <c r="B21" t="n">
-        <v>-1.202622439993756e-05</v>
-      </c>
-      <c r="C21" t="n">
-        <v>53.27214761449191</v>
-      </c>
-      <c r="D21" t="n">
-        <v>87.01688811700902</v>
-      </c>
-      <c r="E21" t="n">
-        <v>771.6850418908354</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1.792540047778188</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.2944088520743037</v>
-      </c>
-      <c r="H21" t="n">
-        <v>125</v>
+      <c r="B22" t="n">
+        <v>-5.169729113274791e-06</v>
+      </c>
+      <c r="C22" t="n">
+        <v>53.27214888613018</v>
+      </c>
+      <c r="D22" t="n">
+        <v>90.54075027739067</v>
+      </c>
+      <c r="E22" t="n">
+        <v>772.2290571380361</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.072497289392378</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.8369189191930244</v>
+      </c>
+      <c r="H22" t="n">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated setup.py to include SciencePlots and resolved findFont warning by just allowing standard font to be used.
</commit_message>
<xml_diff>
--- a/publication/analyses/outputs/field_dependent_effects/gdpt_fit_results.xlsx
+++ b/publication/analyses/outputs/field_dependent_effects/gdpt_fit_results.xlsx
@@ -480,10 +480,10 @@
         <v>-48.09999999999999</v>
       </c>
       <c r="B2" t="n">
-        <v>2.807354666391959e-06</v>
+        <v>2.807354754517037e-06</v>
       </c>
       <c r="C2" t="n">
-        <v>-47.80828328439721</v>
+        <v>-47.80828328181186</v>
       </c>
       <c r="D2" t="n">
         <v>90.82539594511528</v>
@@ -492,10 +492,10 @@
         <v>827.8255058766849</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7416187780432135</v>
+        <v>0.7416187784698118</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4522771597791028</v>
+        <v>0.4522771574658174</v>
       </c>
       <c r="H2" t="n">
         <v>36</v>
@@ -506,10 +506,10 @@
         <v>-43.09999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>2.318331704237215e-06</v>
+        <v>2.318332239370079e-06</v>
       </c>
       <c r="C3" t="n">
-        <v>-43.1463581034952</v>
+        <v>-43.14635836850329</v>
       </c>
       <c r="D3" t="n">
         <v>91.0687371765809</v>
@@ -518,10 +518,10 @@
         <v>827.6612304733294</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8247158227337623</v>
+        <v>0.82471582118389</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7149604747620724</v>
+        <v>0.7149605179054992</v>
       </c>
       <c r="H3" t="n">
         <v>50</v>
@@ -532,10 +532,10 @@
         <v>-38.09999999999999</v>
       </c>
       <c r="B4" t="n">
-        <v>1.997583649813603e-06</v>
+        <v>1.997584378184715e-06</v>
       </c>
       <c r="C4" t="n">
-        <v>-37.68519009447498</v>
+        <v>-37.68519041376937</v>
       </c>
       <c r="D4" t="n">
         <v>90.78470942882738</v>
@@ -544,10 +544,10 @@
         <v>828.8377067354797</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6584143113790158</v>
+        <v>0.6584143330202563</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7484439906196183</v>
+        <v>0.7484440487104622</v>
       </c>
       <c r="H4" t="n">
         <v>66</v>
@@ -558,10 +558,10 @@
         <v>-33.09999999999999</v>
       </c>
       <c r="B5" t="n">
-        <v>2.123850107687925e-06</v>
+        <v>2.123856145547315e-06</v>
       </c>
       <c r="C5" t="n">
-        <v>-32.98388033237012</v>
+        <v>-32.98388251965223</v>
       </c>
       <c r="D5" t="n">
         <v>90.90222861986571</v>
@@ -570,10 +570,10 @@
         <v>829.8173284104438</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9791104742722483</v>
+        <v>0.9791108496116329</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6965302381555001</v>
+        <v>0.6965306036955392</v>
       </c>
       <c r="H5" t="n">
         <v>93</v>
@@ -584,10 +584,10 @@
         <v>-28.09999999999999</v>
       </c>
       <c r="B6" t="n">
-        <v>1.370316348846493e-06</v>
+        <v>1.370333310583349e-06</v>
       </c>
       <c r="C6" t="n">
-        <v>-28.40995576474832</v>
+        <v>-28.40996244040845</v>
       </c>
       <c r="D6" t="n">
         <v>90.65356287048206</v>
@@ -596,10 +596,10 @@
         <v>830.2837598993303</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7939871570038342</v>
+        <v>0.7939887884212922</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6679291470221939</v>
+        <v>0.6679297042232022</v>
       </c>
       <c r="H6" t="n">
         <v>102</v>
@@ -610,10 +610,10 @@
         <v>-23.09999999999999</v>
       </c>
       <c r="B7" t="n">
-        <v>1.336500682314048e-06</v>
+        <v>1.336500357969533e-06</v>
       </c>
       <c r="C7" t="n">
-        <v>-22.86769740813532</v>
+        <v>-22.86769733400465</v>
       </c>
       <c r="D7" t="n">
         <v>90.49122637440026</v>
@@ -622,10 +622,10 @@
         <v>830.6334606269025</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8056979935416008</v>
+        <v>0.8056979796697442</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6697773360623078</v>
+        <v>0.6697773185432365</v>
       </c>
       <c r="H7" t="n">
         <v>93</v>
@@ -636,10 +636,10 @@
         <v>-18.09999999999999</v>
       </c>
       <c r="B8" t="n">
-        <v>6.339377330505732e-07</v>
+        <v>6.339379717368802e-07</v>
       </c>
       <c r="C8" t="n">
-        <v>-18.20520396847115</v>
+        <v>-18.20520396538731</v>
       </c>
       <c r="D8" t="n">
         <v>90.31453946716641</v>
@@ -648,10 +648,10 @@
         <v>830.7242974601622</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9503593593633981</v>
+        <v>0.950359358360359</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5999388612445633</v>
+        <v>0.5999388483716616</v>
       </c>
       <c r="H8" t="n">
         <v>109</v>
@@ -662,10 +662,10 @@
         <v>-13.09999999999999</v>
       </c>
       <c r="B9" t="n">
-        <v>-3.923292934139066e-07</v>
+        <v>-3.923288617649162e-07</v>
       </c>
       <c r="C9" t="n">
-        <v>-13.53538230868667</v>
+        <v>-13.53538236173275</v>
       </c>
       <c r="D9" t="n">
         <v>90.40648246556162</v>
@@ -674,10 +674,10 @@
         <v>831.0423878309792</v>
       </c>
       <c r="F9" t="n">
-        <v>1.291263201793966</v>
+        <v>1.291263223670276</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5191800895904424</v>
+        <v>0.5191800925346544</v>
       </c>
       <c r="H9" t="n">
         <v>118</v>
@@ -688,10 +688,10 @@
         <v>-8.099999999999994</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.201713454144005e-07</v>
+        <v>-2.201733022740605e-07</v>
       </c>
       <c r="C10" t="n">
-        <v>-8.412366981061536</v>
+        <v>-8.412366091911087</v>
       </c>
       <c r="D10" t="n">
         <v>90.13248741757634</v>
@@ -700,10 +700,10 @@
         <v>830.8335811319689</v>
       </c>
       <c r="F10" t="n">
-        <v>1.454015032118664</v>
+        <v>1.454014767604481</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6738613305663195</v>
+        <v>0.6738613683967196</v>
       </c>
       <c r="H10" t="n">
         <v>130</v>
@@ -714,10 +714,10 @@
         <v>-3.099999999999994</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.780561737088979e-06</v>
+        <v>-1.780561784665121e-06</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.162115872956933</v>
+        <v>-4.162115875790266</v>
       </c>
       <c r="D11" t="n">
         <v>186.8533940033314</v>
@@ -726,10 +726,10 @@
         <v>830.5485616267192</v>
       </c>
       <c r="F11" t="n">
-        <v>1.92309375734876</v>
+        <v>1.92309375842447</v>
       </c>
       <c r="G11" t="n">
-        <v>0.617030645028215</v>
+        <v>0.6170306434102218</v>
       </c>
       <c r="H11" t="n">
         <v>110</v>
@@ -740,7 +740,7 @@
         <v>1.900000000000006</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.456425222097137e-06</v>
+        <v>-1.456425122051559e-06</v>
       </c>
       <c r="C12" t="n">
         <v>1.5</v>
@@ -752,10 +752,10 @@
         <v>771.5078743507485</v>
       </c>
       <c r="F12" t="n">
-        <v>2.317933494833103</v>
+        <v>2.317933496773844</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5909648231886309</v>
+        <v>0.5909648223998436</v>
       </c>
       <c r="H12" t="n">
         <v>147</v>
@@ -766,10 +766,10 @@
         <v>6.900000000000006</v>
       </c>
       <c r="B13" t="n">
-        <v>-2.597800555906984e-06</v>
+        <v>-2.5978013873286e-06</v>
       </c>
       <c r="C13" t="n">
-        <v>6.8835898764683</v>
+        <v>6.883590572356017</v>
       </c>
       <c r="D13" t="n">
         <v>90.01028177563565</v>
@@ -778,10 +778,10 @@
         <v>771.6986054665356</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9630761427362112</v>
+        <v>0.9630759390983218</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6927976734993864</v>
+        <v>0.6927977532352302</v>
       </c>
       <c r="H13" t="n">
         <v>108</v>
@@ -792,10 +792,10 @@
         <v>11.90000000000001</v>
       </c>
       <c r="B14" t="n">
-        <v>-3.972583134558911e-06</v>
+        <v>-3.972581961192482e-06</v>
       </c>
       <c r="C14" t="n">
-        <v>12.29422759721204</v>
+        <v>12.29422626908773</v>
       </c>
       <c r="D14" t="n">
         <v>90.13215442508441</v>
@@ -804,10 +804,10 @@
         <v>771.9591986155116</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8578763285692917</v>
+        <v>0.8578766081552265</v>
       </c>
       <c r="G14" t="n">
-        <v>0.730013737971527</v>
+        <v>0.730013798289961</v>
       </c>
       <c r="H14" t="n">
         <v>113</v>
@@ -818,10 +818,10 @@
         <v>16.90000000000001</v>
       </c>
       <c r="B15" t="n">
-        <v>-4.150224890848237e-06</v>
+        <v>-4.150224873790778e-06</v>
       </c>
       <c r="C15" t="n">
-        <v>17.00709991497616</v>
+        <v>17.0070999131628</v>
       </c>
       <c r="D15" t="n">
         <v>90.11881280976174</v>
@@ -830,10 +830,10 @@
         <v>830.6407109746081</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9094924727113068</v>
+        <v>0.9094924730918977</v>
       </c>
       <c r="G15" t="n">
-        <v>0.6966722901866106</v>
+        <v>0.6966722893034571</v>
       </c>
       <c r="H15" t="n">
         <v>121</v>
@@ -844,10 +844,10 @@
         <v>21.90000000000001</v>
       </c>
       <c r="B16" t="n">
-        <v>-4.74171219759843e-06</v>
+        <v>-4.741711141936419e-06</v>
       </c>
       <c r="C16" t="n">
-        <v>22.14348801756694</v>
+        <v>22.14348743371205</v>
       </c>
       <c r="D16" t="n">
         <v>90.21794785462249</v>
@@ -856,10 +856,10 @@
         <v>830.2221608451788</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8859618433942139</v>
+        <v>0.8859619180740933</v>
       </c>
       <c r="G16" t="n">
-        <v>0.7446764198675334</v>
+        <v>0.7446763439093016</v>
       </c>
       <c r="H16" t="n">
         <v>129</v>
@@ -870,10 +870,10 @@
         <v>26.90000000000001</v>
       </c>
       <c r="B17" t="n">
-        <v>-5.359082935497054e-06</v>
+        <v>-5.359082943042832e-06</v>
       </c>
       <c r="C17" t="n">
-        <v>27.84518183297602</v>
+        <v>27.84518183586112</v>
       </c>
       <c r="D17" t="n">
         <v>90.18888841688099</v>
@@ -882,10 +882,10 @@
         <v>829.7983117699556</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8296708481911284</v>
+        <v>0.8296708476706395</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7849704390603754</v>
+        <v>0.7849704395857222</v>
       </c>
       <c r="H17" t="n">
         <v>110</v>
@@ -896,10 +896,10 @@
         <v>31.90000000000001</v>
       </c>
       <c r="B18" t="n">
-        <v>-5.749188649792648e-06</v>
+        <v>-5.749181234521086e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>32.63277172154562</v>
+        <v>32.6327671159276</v>
       </c>
       <c r="D18" t="n">
         <v>90.15951874917874</v>
@@ -908,10 +908,10 @@
         <v>772.4037783531151</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8516371816816438</v>
+        <v>0.8516382208220387</v>
       </c>
       <c r="G18" t="n">
-        <v>0.8454017223418134</v>
+        <v>0.8454009709064916</v>
       </c>
       <c r="H18" t="n">
         <v>105</v>
@@ -922,10 +922,10 @@
         <v>36.90000000000001</v>
       </c>
       <c r="B19" t="n">
-        <v>-6.353635086456746e-06</v>
+        <v>-6.353653790249259e-06</v>
       </c>
       <c r="C19" t="n">
-        <v>37.69291322976677</v>
+        <v>37.69292631788438</v>
       </c>
       <c r="D19" t="n">
         <v>90.29657357722289</v>
@@ -934,10 +934,10 @@
         <v>773.0103223849046</v>
       </c>
       <c r="F19" t="n">
-        <v>1.018444682418053</v>
+        <v>1.018441612666303</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8347642118809966</v>
+        <v>0.8347661573070664</v>
       </c>
       <c r="H19" t="n">
         <v>99</v>
@@ -948,10 +948,10 @@
         <v>41.90000000000001</v>
       </c>
       <c r="B20" t="n">
-        <v>-5.173322225943832e-06</v>
+        <v>-5.173322227183885e-06</v>
       </c>
       <c r="C20" t="n">
-        <v>42.43896634641209</v>
+        <v>42.43896634748508</v>
       </c>
       <c r="D20" t="n">
         <v>89.88634796144834</v>
@@ -960,10 +960,10 @@
         <v>772.4977024774959</v>
       </c>
       <c r="F20" t="n">
-        <v>1.054231890468356</v>
+        <v>1.054231890496467</v>
       </c>
       <c r="G20" t="n">
-        <v>0.7408134193268774</v>
+        <v>0.7408134193996569</v>
       </c>
       <c r="H20" t="n">
         <v>59</v>
@@ -974,10 +974,10 @@
         <v>46.90000000000001</v>
       </c>
       <c r="B21" t="n">
-        <v>-4.696860706679099e-06</v>
+        <v>-4.696848430930113e-06</v>
       </c>
       <c r="C21" t="n">
-        <v>47.73906567743066</v>
+        <v>47.7390566550323</v>
       </c>
       <c r="D21" t="n">
         <v>90.42234393547059</v>
@@ -986,10 +986,10 @@
         <v>772.6022991595236</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8897302893914645</v>
+        <v>0.8897301136663737</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6814896056496886</v>
+        <v>0.6814881549715008</v>
       </c>
       <c r="H21" t="n">
         <v>42</v>
@@ -1000,10 +1000,10 @@
         <v>51.90000000000001</v>
       </c>
       <c r="B22" t="n">
-        <v>-5.169730132685889e-06</v>
+        <v>-5.169730202215532e-06</v>
       </c>
       <c r="C22" t="n">
-        <v>53.27214946097494</v>
+        <v>53.27214947375981</v>
       </c>
       <c r="D22" t="n">
         <v>90.54075027739067</v>
@@ -1012,10 +1012,10 @@
         <v>772.2290571380361</v>
       </c>
       <c r="F22" t="n">
-        <v>1.072497217995571</v>
+        <v>1.072497216412321</v>
       </c>
       <c r="G22" t="n">
-        <v>0.8369190046515274</v>
+        <v>0.8369190037843449</v>
       </c>
       <c r="H22" t="n">
         <v>37</v>

</xml_diff>